<commit_message>
Driver Script file updated
</commit_message>
<xml_diff>
--- a/bin/com/packagename/xlsmain/Login_Verification.xlsx
+++ b/bin/com/packagename/xlsmain/Login_Verification.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Automation-Test\NewWorkspace_2\HybridFramework_1\src\com\packagename\xls\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15900" windowHeight="5625"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase" sheetId="1" r:id="rId1"/>
     <sheet name="TestSteps" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:J16"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,45 +21,129 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="41">
   <si>
     <t>Runmode</t>
   </si>
   <si>
-    <t>Login_Verification</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Admin - Login Check</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Admin - Login Check Parent </t>
-  </si>
-  <si>
-    <t>Admin - Login Check N</t>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>Check email address is able to login to system</t>
+  </si>
+  <si>
+    <t>Check password is able to login to system</t>
+  </si>
+  <si>
+    <t>Check existing customer is able to login to system</t>
+  </si>
+  <si>
+    <t>TSID</t>
+  </si>
+  <si>
+    <t>Keyword</t>
+  </si>
+  <si>
+    <t>Object</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Proceed_on_Fail</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>TS01</t>
+  </si>
+  <si>
+    <t>Open browser</t>
+  </si>
+  <si>
+    <t>OpenWebSite</t>
+  </si>
+  <si>
+    <t>config|testURL</t>
+  </si>
+  <si>
+    <t>TS02</t>
+  </si>
+  <si>
+    <t>click on Sign button</t>
+  </si>
+  <si>
+    <t>clickLink</t>
+  </si>
+  <si>
+    <t>sign_lnk</t>
+  </si>
+  <si>
+    <t>TS03</t>
+  </si>
+  <si>
+    <t>enter user name</t>
+  </si>
+  <si>
+    <t>writeInInput</t>
+  </si>
+  <si>
+    <t>username_Txt</t>
+  </si>
+  <si>
+    <t>config|username</t>
+  </si>
+  <si>
+    <t>TS04</t>
+  </si>
+  <si>
+    <t>click next</t>
+  </si>
+  <si>
+    <t>next_lnk</t>
+  </si>
+  <si>
+    <t>openBrowser</t>
+  </si>
+  <si>
+    <t>config|browserType</t>
+  </si>
+  <si>
+    <t>Navigate to Url</t>
+  </si>
+  <si>
+    <t>navigate</t>
+  </si>
+  <si>
+    <t>click on login button</t>
+  </si>
+  <si>
+    <t>loginlnk_HomePg</t>
+  </si>
+  <si>
+    <t>Login_correct_credentials</t>
+  </si>
+  <si>
+    <t>Login_incorrect_emailaddress</t>
+  </si>
+  <si>
+    <t>Login_incorrect_password</t>
+  </si>
+  <si>
+    <t>Login_delete_customers</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
-    <t>TCID</t>
-  </si>
-  <si>
-    <t>SuperAdmin - Login Check</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parent - Login Check Parent </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Student - login Check </t>
-  </si>
-  <si>
-    <t>Teacher - Login Check</t>
+    <t>Deleted customer verification</t>
   </si>
 </sst>
 </file>
@@ -79,7 +159,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -89,6 +169,23 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -120,9 +217,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,10 +518,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -429,101 +529,46 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
         <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -534,14 +579,242 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="31.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="30.85546875" customWidth="1"/>
+    <col min="7" max="7" width="33.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>